<commit_message>
Update new file and code
</commit_message>
<xml_diff>
--- a/ID3_bagging_nonImput_tabel_matrik.xlsx
+++ b/ID3_bagging_nonImput_tabel_matrik.xlsx
@@ -473,16 +473,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -496,13 +496,13 @@
         <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -516,13 +516,13 @@
         <v>9</v>
       </c>
       <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" t="n">
         <v>18</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -533,16 +533,16 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
@@ -553,16 +553,16 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
-        <v>45</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -573,16 +573,16 @@
         <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -593,16 +593,16 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E8" t="n">
         <v>6</v>
       </c>
       <c r="F8" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="n">
         <v>18</v>
-      </c>
-      <c r="E9" t="n">
-        <v>4</v>
-      </c>
-      <c r="F9" t="n">
-        <v>46</v>
       </c>
     </row>
     <row r="10">
@@ -636,13 +636,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -656,13 +656,13 @@
         <v>9</v>
       </c>
       <c r="D11" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -676,13 +676,13 @@
         <v>9</v>
       </c>
       <c r="D12" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -693,16 +693,16 @@
         <v>13</v>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
-        <v>45</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
@@ -713,16 +713,16 @@
         <v>14</v>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
@@ -733,16 +733,16 @@
         <v>15</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
@@ -753,16 +753,16 @@
         <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
@@ -776,13 +776,13 @@
         <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
@@ -793,16 +793,16 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
@@ -813,16 +813,16 @@
         <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20">
@@ -833,16 +833,16 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -856,13 +856,13 @@
         <v>6</v>
       </c>
       <c r="D21" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E21" t="n">
         <v>2</v>
       </c>
       <c r="F21" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
@@ -873,16 +873,16 @@
         <v>8</v>
       </c>
       <c r="C22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
@@ -896,13 +896,13 @@
         <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -913,16 +913,16 @@
         <v>10</v>
       </c>
       <c r="C24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25">
@@ -933,16 +933,16 @@
         <v>11</v>
       </c>
       <c r="C25" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26">
@@ -953,16 +953,16 @@
         <v>12</v>
       </c>
       <c r="C26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27">
@@ -976,13 +976,13 @@
         <v>5</v>
       </c>
       <c r="D27" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
@@ -993,16 +993,16 @@
         <v>14</v>
       </c>
       <c r="C28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29">
@@ -1013,16 +1013,16 @@
         <v>15</v>
       </c>
       <c r="C29" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30">
@@ -1033,16 +1033,16 @@
         <v>2</v>
       </c>
       <c r="C30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31">
@@ -1053,16 +1053,16 @@
         <v>3</v>
       </c>
       <c r="C31" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D31" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32">
@@ -1073,16 +1073,16 @@
         <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D32" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E32" t="n">
         <v>4</v>
       </c>
       <c r="F32" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33">
@@ -1093,16 +1093,16 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D33" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34">
@@ -1113,16 +1113,16 @@
         <v>6</v>
       </c>
       <c r="C34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35">
@@ -1133,16 +1133,16 @@
         <v>7</v>
       </c>
       <c r="C35" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D35" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36">
@@ -1153,16 +1153,16 @@
         <v>8</v>
       </c>
       <c r="C36" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F36" t="n">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37">
@@ -1173,16 +1173,16 @@
         <v>9</v>
       </c>
       <c r="C37" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D37" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38">
@@ -1193,16 +1193,16 @@
         <v>10</v>
       </c>
       <c r="C38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E38" t="n">
         <v>3</v>
       </c>
       <c r="F38" t="n">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39">
@@ -1213,16 +1213,16 @@
         <v>11</v>
       </c>
       <c r="C39" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D39" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40">
@@ -1233,16 +1233,16 @@
         <v>12</v>
       </c>
       <c r="C40" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D40" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41">
@@ -1253,16 +1253,16 @@
         <v>13</v>
       </c>
       <c r="C41" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D41" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E41" t="n">
         <v>4</v>
       </c>
       <c r="F41" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42">
@@ -1273,16 +1273,16 @@
         <v>14</v>
       </c>
       <c r="C42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D42" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43">
@@ -1293,16 +1293,16 @@
         <v>15</v>
       </c>
       <c r="C43" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D43" t="n">
+        <v>7</v>
+      </c>
+      <c r="E43" t="n">
+        <v>5</v>
+      </c>
+      <c r="F43" t="n">
         <v>22</v>
-      </c>
-      <c r="E43" t="n">
-        <v>4</v>
-      </c>
-      <c r="F43" t="n">
-        <v>46</v>
       </c>
     </row>
     <row r="44">
@@ -1316,13 +1316,13 @@
         <v>4</v>
       </c>
       <c r="D44" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45">
@@ -1333,16 +1333,16 @@
         <v>3</v>
       </c>
       <c r="C45" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D45" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46">
@@ -1353,16 +1353,16 @@
         <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D46" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47">
@@ -1373,16 +1373,16 @@
         <v>5</v>
       </c>
       <c r="C47" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D47" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48">
@@ -1393,16 +1393,16 @@
         <v>6</v>
       </c>
       <c r="C48" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D48" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49">
@@ -1413,16 +1413,16 @@
         <v>7</v>
       </c>
       <c r="C49" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D49" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50">
@@ -1433,16 +1433,16 @@
         <v>8</v>
       </c>
       <c r="C50" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D50" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51">
@@ -1453,16 +1453,16 @@
         <v>9</v>
       </c>
       <c r="C51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D51" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52">
@@ -1473,16 +1473,16 @@
         <v>10</v>
       </c>
       <c r="C52" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D52" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53">
@@ -1493,16 +1493,16 @@
         <v>11</v>
       </c>
       <c r="C53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D53" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54">
@@ -1516,13 +1516,13 @@
         <v>3</v>
       </c>
       <c r="D54" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55">
@@ -1533,16 +1533,16 @@
         <v>13</v>
       </c>
       <c r="C55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D55" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56">
@@ -1556,13 +1556,13 @@
         <v>4</v>
       </c>
       <c r="D56" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57">
@@ -1573,16 +1573,16 @@
         <v>15</v>
       </c>
       <c r="C57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E57" t="n">
         <v>5</v>
       </c>
       <c r="F57" t="n">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58">
@@ -1593,16 +1593,16 @@
         <v>2</v>
       </c>
       <c r="C58" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D58" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59">
@@ -1613,16 +1613,16 @@
         <v>3</v>
       </c>
       <c r="C59" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D59" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60">
@@ -1633,16 +1633,16 @@
         <v>4</v>
       </c>
       <c r="C60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D60" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E60" t="n">
         <v>5</v>
       </c>
       <c r="F60" t="n">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61">
@@ -1653,16 +1653,16 @@
         <v>5</v>
       </c>
       <c r="C61" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D61" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="E61" t="n">
         <v>4</v>
       </c>
       <c r="F61" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62">
@@ -1676,13 +1676,13 @@
         <v>5</v>
       </c>
       <c r="D62" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E62" t="n">
         <v>6</v>
       </c>
       <c r="F62" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63">
@@ -1693,16 +1693,16 @@
         <v>7</v>
       </c>
       <c r="C63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D63" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64">
@@ -1713,16 +1713,16 @@
         <v>8</v>
       </c>
       <c r="C64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D64" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65">
@@ -1736,13 +1736,13 @@
         <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66">
@@ -1753,16 +1753,16 @@
         <v>10</v>
       </c>
       <c r="C66" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D66" t="n">
+        <v>9</v>
+      </c>
+      <c r="E66" t="n">
+        <v>5</v>
+      </c>
+      <c r="F66" t="n">
         <v>21</v>
-      </c>
-      <c r="E66" t="n">
-        <v>5</v>
-      </c>
-      <c r="F66" t="n">
-        <v>45</v>
       </c>
     </row>
     <row r="67">
@@ -1773,16 +1773,16 @@
         <v>11</v>
       </c>
       <c r="C67" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D67" t="n">
+        <v>8</v>
+      </c>
+      <c r="E67" t="n">
+        <v>2</v>
+      </c>
+      <c r="F67" t="n">
         <v>24</v>
-      </c>
-      <c r="E67" t="n">
-        <v>4</v>
-      </c>
-      <c r="F67" t="n">
-        <v>46</v>
       </c>
     </row>
     <row r="68">
@@ -1793,16 +1793,16 @@
         <v>12</v>
       </c>
       <c r="C68" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D68" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E68" t="n">
         <v>5</v>
       </c>
       <c r="F68" t="n">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69">
@@ -1816,13 +1816,13 @@
         <v>6</v>
       </c>
       <c r="D69" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70">
@@ -1833,16 +1833,16 @@
         <v>14</v>
       </c>
       <c r="C70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D70" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="71">
@@ -1853,16 +1853,16 @@
         <v>15</v>
       </c>
       <c r="C71" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D71" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72">
@@ -1873,16 +1873,16 @@
         <v>2</v>
       </c>
       <c r="C72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D72" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73">
@@ -1893,16 +1893,16 @@
         <v>3</v>
       </c>
       <c r="C73" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D73" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74">
@@ -1913,16 +1913,16 @@
         <v>4</v>
       </c>
       <c r="C74" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D74" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75">
@@ -1933,16 +1933,16 @@
         <v>5</v>
       </c>
       <c r="C75" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D75" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76">
@@ -1953,16 +1953,16 @@
         <v>6</v>
       </c>
       <c r="C76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D76" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E76" t="n">
         <v>7</v>
       </c>
       <c r="F76" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77">
@@ -1973,16 +1973,16 @@
         <v>7</v>
       </c>
       <c r="C77" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E77" t="n">
         <v>6</v>
       </c>
       <c r="F77" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78">
@@ -1993,16 +1993,16 @@
         <v>8</v>
       </c>
       <c r="C78" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D78" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E78" t="n">
         <v>6</v>
       </c>
       <c r="F78" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79">
@@ -2013,16 +2013,16 @@
         <v>9</v>
       </c>
       <c r="C79" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D79" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E79" t="n">
         <v>6</v>
       </c>
       <c r="F79" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80">
@@ -2036,13 +2036,13 @@
         <v>5</v>
       </c>
       <c r="D80" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81">
@@ -2056,13 +2056,13 @@
         <v>6</v>
       </c>
       <c r="D81" t="n">
+        <v>7</v>
+      </c>
+      <c r="E81" t="n">
+        <v>5</v>
+      </c>
+      <c r="F81" t="n">
         <v>21</v>
-      </c>
-      <c r="E81" t="n">
-        <v>5</v>
-      </c>
-      <c r="F81" t="n">
-        <v>45</v>
       </c>
     </row>
     <row r="82">
@@ -2073,16 +2073,16 @@
         <v>12</v>
       </c>
       <c r="C82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D82" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83">
@@ -2096,13 +2096,13 @@
         <v>7</v>
       </c>
       <c r="D83" t="n">
+        <v>6</v>
+      </c>
+      <c r="E83" t="n">
+        <v>6</v>
+      </c>
+      <c r="F83" t="n">
         <v>20</v>
-      </c>
-      <c r="E83" t="n">
-        <v>7</v>
-      </c>
-      <c r="F83" t="n">
-        <v>43</v>
       </c>
     </row>
     <row r="84">
@@ -2113,16 +2113,16 @@
         <v>14</v>
       </c>
       <c r="C84" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D84" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85">
@@ -2133,16 +2133,16 @@
         <v>15</v>
       </c>
       <c r="C85" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D85" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E85" t="n">
         <v>6</v>
       </c>
       <c r="F85" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86">
@@ -2153,16 +2153,16 @@
         <v>2</v>
       </c>
       <c r="C86" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D86" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87">
@@ -2176,13 +2176,13 @@
         <v>4</v>
       </c>
       <c r="D87" t="n">
+        <v>9</v>
+      </c>
+      <c r="E87" t="n">
+        <v>3</v>
+      </c>
+      <c r="F87" t="n">
         <v>23</v>
-      </c>
-      <c r="E87" t="n">
-        <v>4</v>
-      </c>
-      <c r="F87" t="n">
-        <v>46</v>
       </c>
     </row>
     <row r="88">
@@ -2193,16 +2193,16 @@
         <v>4</v>
       </c>
       <c r="C88" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D88" t="n">
+        <v>8</v>
+      </c>
+      <c r="E88" t="n">
+        <v>6</v>
+      </c>
+      <c r="F88" t="n">
         <v>20</v>
-      </c>
-      <c r="E88" t="n">
-        <v>2</v>
-      </c>
-      <c r="F88" t="n">
-        <v>48</v>
       </c>
     </row>
     <row r="89">
@@ -2213,16 +2213,16 @@
         <v>5</v>
       </c>
       <c r="C89" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D89" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90">
@@ -2233,16 +2233,16 @@
         <v>6</v>
       </c>
       <c r="C90" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D90" t="n">
+        <v>8</v>
+      </c>
+      <c r="E90" t="n">
+        <v>3</v>
+      </c>
+      <c r="F90" t="n">
         <v>23</v>
-      </c>
-      <c r="E90" t="n">
-        <v>2</v>
-      </c>
-      <c r="F90" t="n">
-        <v>48</v>
       </c>
     </row>
     <row r="91">
@@ -2253,16 +2253,16 @@
         <v>7</v>
       </c>
       <c r="C91" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D91" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E91" t="n">
         <v>3</v>
       </c>
       <c r="F91" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92">
@@ -2273,16 +2273,16 @@
         <v>8</v>
       </c>
       <c r="C92" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D92" t="n">
+        <v>9</v>
+      </c>
+      <c r="E92" t="n">
+        <v>5</v>
+      </c>
+      <c r="F92" t="n">
         <v>21</v>
-      </c>
-      <c r="E92" t="n">
-        <v>3</v>
-      </c>
-      <c r="F92" t="n">
-        <v>47</v>
       </c>
     </row>
     <row r="93">
@@ -2296,13 +2296,13 @@
         <v>8</v>
       </c>
       <c r="D93" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E93" t="n">
         <v>4</v>
       </c>
       <c r="F93" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94">
@@ -2313,16 +2313,16 @@
         <v>10</v>
       </c>
       <c r="C94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D94" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95">
@@ -2333,16 +2333,16 @@
         <v>11</v>
       </c>
       <c r="C95" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D95" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96">
@@ -2353,16 +2353,16 @@
         <v>12</v>
       </c>
       <c r="C96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D96" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97">
@@ -2373,16 +2373,16 @@
         <v>13</v>
       </c>
       <c r="C97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D97" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E97" t="n">
         <v>4</v>
       </c>
       <c r="F97" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98">
@@ -2396,13 +2396,13 @@
         <v>6</v>
       </c>
       <c r="D98" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99">
@@ -2413,16 +2413,16 @@
         <v>15</v>
       </c>
       <c r="C99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D99" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E99" t="n">
         <v>3</v>
       </c>
       <c r="F99" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100">
@@ -2433,16 +2433,16 @@
         <v>2</v>
       </c>
       <c r="C100" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D100" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E100" t="n">
         <v>6</v>
       </c>
       <c r="F100" t="n">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101">
@@ -2453,16 +2453,16 @@
         <v>3</v>
       </c>
       <c r="C101" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D101" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E101" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F101" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102">
@@ -2476,13 +2476,13 @@
         <v>7</v>
       </c>
       <c r="D102" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E102" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F102" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="103">
@@ -2493,16 +2493,16 @@
         <v>5</v>
       </c>
       <c r="C103" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D103" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E103" t="n">
         <v>5</v>
       </c>
       <c r="F103" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="104">
@@ -2513,16 +2513,16 @@
         <v>6</v>
       </c>
       <c r="C104" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D104" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E104" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F104" t="n">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105">
@@ -2536,13 +2536,13 @@
         <v>8</v>
       </c>
       <c r="D105" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E105" t="n">
         <v>4</v>
       </c>
       <c r="F105" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106">
@@ -2553,16 +2553,16 @@
         <v>8</v>
       </c>
       <c r="C106" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D106" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E106" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F106" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="107">
@@ -2576,13 +2576,13 @@
         <v>8</v>
       </c>
       <c r="D107" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E107" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F107" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108">
@@ -2593,16 +2593,16 @@
         <v>10</v>
       </c>
       <c r="C108" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D108" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E108" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F108" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="109">
@@ -2613,16 +2613,16 @@
         <v>11</v>
       </c>
       <c r="C109" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D109" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E109" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F109" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="110">
@@ -2633,16 +2633,16 @@
         <v>12</v>
       </c>
       <c r="C110" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D110" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E110" t="n">
         <v>3</v>
       </c>
       <c r="F110" t="n">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111">
@@ -2653,16 +2653,16 @@
         <v>13</v>
       </c>
       <c r="C111" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D111" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E111" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F111" t="n">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="112">
@@ -2673,16 +2673,16 @@
         <v>14</v>
       </c>
       <c r="C112" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D112" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E112" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F112" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113">
@@ -2693,16 +2693,16 @@
         <v>15</v>
       </c>
       <c r="C113" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D113" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E113" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F113" t="n">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="114">
@@ -2713,16 +2713,16 @@
         <v>2</v>
       </c>
       <c r="C114" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D114" t="n">
+        <v>4</v>
+      </c>
+      <c r="E114" t="n">
+        <v>3</v>
+      </c>
+      <c r="F114" t="n">
         <v>23</v>
-      </c>
-      <c r="E114" t="n">
-        <v>7</v>
-      </c>
-      <c r="F114" t="n">
-        <v>43</v>
       </c>
     </row>
     <row r="115">
@@ -2733,16 +2733,16 @@
         <v>3</v>
       </c>
       <c r="C115" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D115" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E115" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F115" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116">
@@ -2753,16 +2753,16 @@
         <v>4</v>
       </c>
       <c r="C116" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D116" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E116" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F116" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="117">
@@ -2776,13 +2776,13 @@
         <v>6</v>
       </c>
       <c r="D117" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E117" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F117" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118">
@@ -2793,16 +2793,16 @@
         <v>6</v>
       </c>
       <c r="C118" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D118" t="n">
+        <v>5</v>
+      </c>
+      <c r="E118" t="n">
+        <v>5</v>
+      </c>
+      <c r="F118" t="n">
         <v>21</v>
-      </c>
-      <c r="E118" t="n">
-        <v>6</v>
-      </c>
-      <c r="F118" t="n">
-        <v>44</v>
       </c>
     </row>
     <row r="119">
@@ -2816,13 +2816,13 @@
         <v>7</v>
       </c>
       <c r="D119" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E119" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F119" t="n">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="120">
@@ -2833,16 +2833,16 @@
         <v>8</v>
       </c>
       <c r="C120" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D120" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E120" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F120" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="121">
@@ -2853,16 +2853,16 @@
         <v>9</v>
       </c>
       <c r="C121" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D121" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E121" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F121" t="n">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="122">
@@ -2873,16 +2873,16 @@
         <v>10</v>
       </c>
       <c r="C122" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D122" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E122" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F122" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="123">
@@ -2893,16 +2893,16 @@
         <v>11</v>
       </c>
       <c r="C123" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D123" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E123" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F123" t="n">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124">
@@ -2913,16 +2913,16 @@
         <v>12</v>
       </c>
       <c r="C124" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D124" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E124" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F124" t="n">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="125">
@@ -2936,13 +2936,13 @@
         <v>5</v>
       </c>
       <c r="D125" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E125" t="n">
         <v>6</v>
       </c>
       <c r="F125" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126">
@@ -2956,13 +2956,13 @@
         <v>6</v>
       </c>
       <c r="D126" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E126" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F126" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="127">
@@ -2973,16 +2973,16 @@
         <v>15</v>
       </c>
       <c r="C127" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D127" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E127" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F127" t="n">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="128">
@@ -2993,16 +2993,16 @@
         <v>2</v>
       </c>
       <c r="C128" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D128" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E128" t="n">
         <v>7</v>
       </c>
       <c r="F128" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="129">
@@ -3013,16 +3013,16 @@
         <v>3</v>
       </c>
       <c r="C129" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D129" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E129" t="n">
         <v>4</v>
       </c>
       <c r="F129" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="130">
@@ -3033,16 +3033,16 @@
         <v>4</v>
       </c>
       <c r="C130" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D130" t="n">
+        <v>9</v>
+      </c>
+      <c r="E130" t="n">
+        <v>2</v>
+      </c>
+      <c r="F130" t="n">
         <v>24</v>
-      </c>
-      <c r="E130" t="n">
-        <v>1</v>
-      </c>
-      <c r="F130" t="n">
-        <v>49</v>
       </c>
     </row>
     <row r="131">
@@ -3053,16 +3053,16 @@
         <v>5</v>
       </c>
       <c r="C131" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D131" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E131" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F131" t="n">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="132">
@@ -3076,13 +3076,13 @@
         <v>3</v>
       </c>
       <c r="D132" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E132" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F132" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="133">
@@ -3093,16 +3093,16 @@
         <v>7</v>
       </c>
       <c r="C133" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D133" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E133" t="n">
         <v>2</v>
       </c>
       <c r="F133" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="134">
@@ -3113,16 +3113,16 @@
         <v>8</v>
       </c>
       <c r="C134" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D134" t="n">
+        <v>8</v>
+      </c>
+      <c r="E134" t="n">
+        <v>3</v>
+      </c>
+      <c r="F134" t="n">
         <v>23</v>
-      </c>
-      <c r="E134" t="n">
-        <v>2</v>
-      </c>
-      <c r="F134" t="n">
-        <v>48</v>
       </c>
     </row>
     <row r="135">
@@ -3133,16 +3133,16 @@
         <v>9</v>
       </c>
       <c r="C135" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D135" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F135" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="136">
@@ -3153,16 +3153,16 @@
         <v>10</v>
       </c>
       <c r="C136" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D136" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E136" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F136" t="n">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="137">
@@ -3176,13 +3176,13 @@
         <v>4</v>
       </c>
       <c r="D137" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E137" t="n">
         <v>2</v>
       </c>
       <c r="F137" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138">
@@ -3193,16 +3193,16 @@
         <v>12</v>
       </c>
       <c r="C138" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D138" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F138" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="139">
@@ -3213,16 +3213,16 @@
         <v>13</v>
       </c>
       <c r="C139" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D139" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F139" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="140">
@@ -3233,16 +3233,16 @@
         <v>14</v>
       </c>
       <c r="C140" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D140" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F140" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="141">
@@ -3253,16 +3253,16 @@
         <v>15</v>
       </c>
       <c r="C141" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D141" t="n">
+        <v>10</v>
+      </c>
+      <c r="E141" t="n">
+        <v>1</v>
+      </c>
+      <c r="F141" t="n">
         <v>25</v>
-      </c>
-      <c r="E141" t="n">
-        <v>0</v>
-      </c>
-      <c r="F141" t="n">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>